<commit_message>
modified program to update MultiplexPCR reports
</commit_message>
<xml_diff>
--- a/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
+++ b/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test_22.7\server\modules\onprcEHRModules\onprc_ehr\resources\web\onprc_ehr\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DCC193-BD19-4922-A810-E6A9A1A51BD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C702F15-C726-4564-B48A-6624CEFDECF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{3C994614-C82B-4F4F-8C34-DAAF4D70F013}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{3C994614-C82B-4F4F-8C34-DAAF4D70F013}"/>
   </bookViews>
   <sheets>
     <sheet name="for GI" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
   <si>
     <t xml:space="preserve"> Detected</t>
   </si>
@@ -343,12 +343,15 @@
   <si>
     <t>Leave blank</t>
   </si>
+  <si>
+    <t>Multiplex PCR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,6 +392,12 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF067D17"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -480,7 +489,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -571,6 +580,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1748,21 +1760,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C928D-1244-458E-8FED-C5008946B38A}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="31" t="s">
         <v>27</v>
       </c>
@@ -1773,7 +1785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
         <v>40</v>
       </c>
@@ -1784,7 +1796,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="28" t="s">
         <v>34</v>
       </c>
@@ -1796,7 +1808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="31" t="s">
         <v>31</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="28" t="s">
         <v>39</v>
       </c>
@@ -1818,12 +1830,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>33</v>
+      <c r="B6" s="37" t="s">
+        <v>53</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>48</v>
@@ -1835,7 +1847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="33" t="s">
         <v>36</v>
       </c>
@@ -1849,7 +1861,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="31" t="s">
         <v>29</v>
       </c>
@@ -1858,47 +1870,47 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1906,119 +1918,119 @@
       <c r="C15" s="10"/>
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="23" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="26.4">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15" thickBot="1">
       <c r="A27" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15" thickBot="1">
       <c r="A32" s="13" t="s">
         <v>24</v>
       </c>
@@ -2051,22 +2063,22 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="22" t="s">
         <v>43</v>
       </c>
@@ -2084,15 +2096,15 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.88671875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -2100,7 +2112,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -2118,7 +2130,7 @@
       <c r="C3" s="20"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2126,7 +2138,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -2142,7 +2154,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="18" t="s">
         <v>36</v>
       </c>
@@ -2153,7 +2165,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2172,7 +2184,7 @@
         <v>35160</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2183,7 +2195,7 @@
         <v>44854.063194444447</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
@@ -2205,7 +2217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -2227,7 +2239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -2238,7 +2250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="19" t="s">
         <v>7</v>
       </c>
@@ -2249,7 +2261,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -2260,7 +2272,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="9" t="s">
         <v>9</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +2294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
@@ -2293,7 +2305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="26.4">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
@@ -2315,7 +2327,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -2326,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2337,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2360,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
@@ -2359,7 +2371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15" thickBot="1">
       <c r="A27" s="7" t="s">
         <v>19</v>
       </c>
@@ -2370,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="9" t="s">
         <v>20</v>
       </c>
@@ -2381,7 +2393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="11" t="s">
         <v>21</v>
       </c>
@@ -2392,7 +2404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
         <v>23</v>
       </c>
@@ -2414,7 +2426,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15" thickBot="1">
       <c r="A32" s="13" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
modified program to include Biofire BC Panel.
</commit_message>
<xml_diff>
--- a/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
+++ b/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test_22.7\server\modules\onprcEHRModules\onprc_ehr\resources\web\onprc_ehr\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\XML_Project\Heidi_Palmer\Final_BioFireTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C702F15-C726-4564-B48A-6624CEFDECF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3C7FB3-4B73-4953-A1D3-BDE613F8D7A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7980" xr2:uid="{3C994614-C82B-4F4F-8C34-DAAF4D70F013}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{3C994614-C82B-4F4F-8C34-DAAF4D70F013}"/>
   </bookViews>
   <sheets>
     <sheet name="for GI" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
   <si>
     <t xml:space="preserve"> Detected</t>
   </si>
@@ -320,9 +320,6 @@
     <t>Detected</t>
   </si>
   <si>
-    <t>Do not need Instrument number</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
@@ -341,10 +338,16 @@
     <t>Tissue=Stool (T-6Y100)</t>
   </si>
   <si>
-    <t>Leave blank</t>
-  </si>
-  <si>
     <t>Multiplex PCR</t>
+  </si>
+  <si>
+    <t>T-6Y100</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Testng for you you.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
     </font>
     <font>
       <sz val="9.8000000000000007"/>
-      <color rgb="FF067D17"/>
+      <color rgb="FF0033B3"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -1758,32 +1761,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C928D-1244-458E-8FED-C5008946B38A}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="31" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="28" t="s">
@@ -1793,7 +1794,7 @@
         <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1805,7 +1806,7 @@
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1816,7 +1817,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1827,24 +1828,24 @@
         <v>492</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>53</v>
+      <c r="B6" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="34" t="s">
         <v>48</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1858,184 +1859,242 @@
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="D8" s="21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="B9" s="27"/>
+      <c r="D9" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>41229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="14">
+        <v>44852.063194444447</v>
+      </c>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="23" t="s">
+      <c r="B16" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="9" t="s">
+      <c r="B18" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="12"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-    </row>
-    <row r="21" spans="1:3" ht="26.4">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:3" ht="25.5">
+      <c r="A22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
-      <c r="A23" s="7" t="s">
+      <c r="B23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
-      <c r="A27" s="7" t="s">
+      <c r="B27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
+      <c r="B29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="10"/>
+        <v>21</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>2</v>
+      </c>
       <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="10"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
-      <c r="A32" s="13" t="s">
+      <c r="B32" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A33" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="B33" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2047,7 +2106,7 @@
           <x14:formula1>
             <xm:f>'cheat sheet'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:C32</xm:sqref>
+          <xm:sqref>B12:C33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2063,9 +2122,9 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -2096,12 +2155,12 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2184,7 +2243,7 @@
         <v>35160</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2261,7 +2320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
@@ -2305,7 +2364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="26.4">
+    <row r="21" spans="1:3" ht="25.5">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -2371,7 +2430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27" s="7" t="s">
         <v>19</v>
       </c>
@@ -2426,7 +2485,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1">
       <c r="A32" s="13" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Modified to update form template files.
</commit_message>
<xml_diff>
--- a/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
+++ b/onprc_ehr/resources/web/onprc_ehr/templates/BioFireTemplate_GI_Panel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\XML_Project\Heidi_Palmer\Final_BioFireTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18CC6CAC-9E5B-4102-8C25-B24C4725A15F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E018229B-C4A1-45A8-BCDB-8F2AACD8834F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{3C994614-C82B-4F4F-8C34-DAAF4D70F013}"/>
   </bookViews>
   <sheets>
     <sheet name="for GI" sheetId="2" r:id="rId1"/>
+    <sheet name="cheat sheet" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,11 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Campylobacter</t>
   </si>
   <si>
+    <t>Not Detected</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Clostridium difficile </t>
     </r>
@@ -291,22 +295,10 @@
     <t>Biofire GI PCR Panel</t>
   </si>
   <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>specific Service Request for each panel</t>
-  </si>
-  <si>
-    <t>Method=Multiplex PCR</t>
-  </si>
-  <si>
-    <t>need separate line for tissue</t>
-  </si>
-  <si>
-    <t>have blank field to enter initials like other templates</t>
-  </si>
-  <si>
-    <t>Tissue=Stool (T-6Y100)</t>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Detected</t>
   </si>
   <si>
     <t>Multiplex PCR</t>
@@ -457,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -492,6 +484,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed" wrapText="1"/>
     </xf>
@@ -846,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6C928D-1244-458E-8FED-C5008946B38A}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -861,112 +854,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="18"/>
+      <c r="A1" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="19"/>
       <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="19" t="s">
+      <c r="B5" s="24">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="26"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="22">
+        <v>2135</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="22" t="s">
+      <c r="B8" s="29"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="23">
-        <v>492</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="21">
-        <v>2135</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="D9" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="B9" s="19"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -980,148 +952,148 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="14" t="s">
-        <v>5</v>
+      <c r="A17" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" ht="25.5">
       <c r="A22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1">
       <c r="A33" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -1134,7 +1106,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F09135B2-0A48-4164-9EA9-21F26A779870}">
           <x14:formula1>
-            <xm:f>#REF!</xm:f>
+            <xm:f>'cheat sheet'!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B12:C33</xm:sqref>
         </x14:dataValidation>
@@ -1142,4 +1114,37 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{890D7E3B-CF8B-46E3-BE5C-A54EC36756A8}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>